<commit_message>
added xlsx data files to data folder
</commit_message>
<xml_diff>
--- a/data/aktie.xlsx
+++ b/data/aktie.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conny\Desktop\Computerlinguistik\Semester 8\Tabellen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E6763F9-2B19-4F31-B9BD-0AC8B46D71B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CAC917E-2888-40D2-A90D-167443C115A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CA97BEE1-AE75-4114-9467-EC2BFE68DD65}"/>
   </bookViews>
@@ -48,20 +48,30 @@
     <t>Dividendenvorschlag</t>
   </si>
   <si>
-    <t>– 0,03</t>
+    <t>– 0.03</t>
   </si>
   <si>
-    <t>– 12,51</t>
+    <t>– 12.51</t>
   </si>
   <si>
-    <t>– 2,99</t>
+    <t>– 2.99</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -87,15 +97,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Währung" xfId="1" builtinId="4"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -410,7 +423,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -433,13 +446,13 @@
       <c r="A2">
         <v>2010</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2">
         <v>16.36</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2">
         <v>2.4700000000000002</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2">
         <v>0.6</v>
       </c>
     </row>
@@ -447,13 +460,13 @@
       <c r="A3">
         <v>2011</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3">
         <v>9.19</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3">
         <v>0.25</v>
       </c>
     </row>
@@ -576,7 +589,7 @@
       <c r="B12">
         <v>10.82</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D12">
@@ -590,7 +603,7 @@
       <c r="B13">
         <v>6.18</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D13">

</xml_diff>

<commit_message>
updated xlsx and csv data files in data folder
</commit_message>
<xml_diff>
--- a/data/aktie.xlsx
+++ b/data/aktie.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conny\Desktop\Computerlinguistik\Semester 8\Tabellen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CAC917E-2888-40D2-A90D-167443C115A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F82333DF-720D-4269-88C4-5F65C83B6A52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CA97BEE1-AE75-4114-9467-EC2BFE68DD65}"/>
   </bookViews>
@@ -36,18 +36,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
-    <t>Jahr</t>
-  </si>
-  <si>
-    <t>Jahresschlusskurs</t>
-  </si>
-  <si>
-    <t>Ergebnis pro Aktie</t>
-  </si>
-  <si>
-    <t>Dividendenvorschlag</t>
-  </si>
-  <si>
     <t>– 0.03</t>
   </si>
   <si>
@@ -55,6 +43,18 @@
   </si>
   <si>
     <t>– 2.99</t>
+  </si>
+  <si>
+    <t>jahr</t>
+  </si>
+  <si>
+    <t>jahresschlusskurs</t>
+  </si>
+  <si>
+    <t>ergebnis_pro_aktie</t>
+  </si>
+  <si>
+    <t>dividendenvorschlag</t>
   </si>
 </sst>
 </file>
@@ -101,10 +101,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -423,23 +422,23 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -463,8 +462,8 @@
       <c r="B3">
         <v>9.19</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>4</v>
+      <c r="C3" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="D3">
         <v>0.25</v>
@@ -590,7 +589,7 @@
         <v>10.82</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -604,7 +603,7 @@
         <v>6.18</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D13">
         <v>0</v>

</xml_diff>